<commit_message>
feat(grid-selenium): add parallel Grid tests with dynamic driver options
- Implemented 'TestGridParallel':
  * Uses a 'ThreadLocal<IWebDriver>' to keep one browser instance per test thread.
  * 'GetBrowserOptions()' returns the proper options object ('ChromeOptions' or 'FirefoxOptions') based on the supplied browser name.
  * 'SetUp()' accepts a 'browserName' parameter, creates a 'RemoteWebDriver' pointing to 'http://localhost:4444', sets the platform, and navigates to Facebook.
  * 'TearDown()' safely quits/disposes the thread‑specific driver.
  * 'LoginTest' is data‑driven: reads username, password and browser from an Excel sheet, invokes 'SetUp(browserName)', performs login, and pauses 5 s.
  * 'GetTestData()' pulls the required columns from 'LoginTest' sheet in 'testdata.xlsx'.

- Adds support for Selenium Grid execution with dynamic browser selection,
  enabling concurrent runs across Chrome and Firefox on the same hub.
</commit_message>
<xml_diff>
--- a/SeleniumAutomation/SeleniumAutomation/resources/testdata.xlsx
+++ b/SeleniumAutomation/SeleniumAutomation/resources/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -29,16 +29,25 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
+    <t xml:space="preserve">browser</t>
+  </si>
+  <si>
     <t xml:space="preserve">trainer@way2automation.com</t>
   </si>
   <si>
     <t xml:space="preserve">sfdsfdsfd</t>
   </si>
   <si>
+    <t xml:space="preserve">chrome</t>
+  </si>
+  <si>
     <t xml:space="preserve">info@way2automation.com</t>
   </si>
   <si>
     <t xml:space="preserve">xfdsfdawdsfd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firefox</t>
   </si>
   <si>
     <t xml:space="preserve">java@way2automation.com</t>
@@ -80,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -101,12 +111,14 @@
       <color rgb="FFA31515"/>
       <name val="Cascadia Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9.5"/>
       <color rgb="FF0000FF"/>
       <name val="Cascadia Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,16 +163,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -347,54 +363,66 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="trainer@way2automation.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="info@way2automation"/>
+    <hyperlink ref="A3" r:id="rId2" display="info@way2automation.com"/>
     <hyperlink ref="A4" r:id="rId3" display="java@way2automation.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -414,42 +442,42 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>9</v>
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>